<commit_message>
Update DR# 610 Veterans Bank(Marikina and Concepcion ICE Cards)_10_02_2020.xlsx
</commit_message>
<xml_diff>
--- a/DR# 610 Veterans Bank(Marikina and Concepcion ICE Cards)_10_02_2020.xlsx
+++ b/DR# 610 Veterans Bank(Marikina and Concepcion ICE Cards)_10_02_2020.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Delivery-Receipt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BCA453B-D81C-41A2-98D4-418D7C68252D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{642BF10D-6ED2-4A0F-92DE-385F02FEA6DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -164,9 +164,6 @@
     <t>Attn To: Ferdinand Ramos</t>
   </si>
   <si>
-    <t>To:  Veterans Bank of the Philippines</t>
-  </si>
-  <si>
     <t>Card</t>
   </si>
   <si>
@@ -174,6 +171,9 @@
   </si>
   <si>
     <t>Brgy. Concepcion UNO ID ICE Card</t>
+  </si>
+  <si>
+    <t>To:  PVB</t>
   </si>
 </sst>
 </file>
@@ -498,6 +498,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -506,12 +512,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -971,13 +971,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1193,13 +1193,13 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1385,8 +1385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="115" zoomScaleNormal="70" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1414,13 +1414,13 @@
       </c>
     </row>
     <row r="7" spans="1:13" ht="50.25" customHeight="1">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
+      <c r="B7" s="46"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
@@ -1446,7 +1446,7 @@
     </row>
     <row r="10" spans="1:13" ht="21" customHeight="1">
       <c r="A10" s="26" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B10" s="26"/>
       <c r="C10" s="26"/>
@@ -1469,21 +1469,21 @@
       <c r="I11" s="2"/>
     </row>
     <row r="12" spans="1:13" ht="21" customHeight="1">
-      <c r="A12" s="45" t="s">
+      <c r="A12" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="46"/>
-      <c r="C12" s="46"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
-      <c r="F12" s="46"/>
-      <c r="G12" s="46"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="46"/>
-      <c r="J12" s="46"/>
-      <c r="K12" s="46"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="46"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
+      <c r="F12" s="48"/>
+      <c r="G12" s="48"/>
+      <c r="H12" s="48"/>
+      <c r="I12" s="48"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="48"/>
+      <c r="L12" s="48"/>
+      <c r="M12" s="48"/>
     </row>
     <row r="13" spans="1:13" ht="18">
       <c r="A13" s="23"/>
@@ -1519,10 +1519,10 @@
     </row>
     <row r="16" spans="1:13" ht="36">
       <c r="A16" s="43" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" s="37" t="s">
         <v>28</v>
-      </c>
-      <c r="B16" s="37" t="s">
-        <v>29</v>
       </c>
       <c r="C16" s="36">
         <v>500</v>
@@ -1535,11 +1535,11 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="36">
-      <c r="A17" s="47" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="48" t="s">
-        <v>30</v>
+      <c r="A17" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="45" t="s">
+        <v>29</v>
       </c>
       <c r="C17" s="29">
         <v>200</v>

</xml_diff>